<commit_message>
Copy all files from DDT-Framework project to do refactoring
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="test_suite" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="RemoveCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AddCustomerTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="OpenAccountTest" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="testSuite" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -48,7 +49,7 @@
     <t xml:space="preserve">Customer added successfully</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
+    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">Maria</t>
@@ -57,16 +58,7 @@
     <t xml:space="preserve">Santos</t>
   </si>
   <si>
-    <t xml:space="preserve">Jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alvez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jorge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Souza</t>
+    <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">customer</t>
@@ -81,10 +73,7 @@
     <t xml:space="preserve">Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">TCID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runmode</t>
+    <t xml:space="preserve">tcid</t>
   </si>
   <si>
     <t xml:space="preserve">BankManagerLoginTest</t>
@@ -175,17 +164,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -209,13 +194,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -268,47 +253,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>123654</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>789456</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -317,6 +268,84 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>654321</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -324,31 +353,31 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
+      <c r="A2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -357,7 +386,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -365,7 +394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -373,38 +402,38 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
+      <c r="A2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
+      <c r="A3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
+      <c r="A4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -413,7 +442,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Copy all files from DDT-Framework project to do refactoring (#4)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="test_suite" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="RemoveCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AddCustomerTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="OpenAccountTest" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="testSuite" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -48,7 +49,7 @@
     <t xml:space="preserve">Customer added successfully</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
+    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">Maria</t>
@@ -57,16 +58,7 @@
     <t xml:space="preserve">Santos</t>
   </si>
   <si>
-    <t xml:space="preserve">Jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alvez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jorge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Souza</t>
+    <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">customer</t>
@@ -81,10 +73,7 @@
     <t xml:space="preserve">Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">TCID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runmode</t>
+    <t xml:space="preserve">tcid</t>
   </si>
   <si>
     <t xml:space="preserve">BankManagerLoginTest</t>
@@ -175,17 +164,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -209,13 +194,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -268,47 +253,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>123654</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>789456</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -317,6 +268,84 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>654321</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -324,31 +353,31 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
+      <c r="A2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -357,7 +386,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -365,7 +394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -373,38 +402,38 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
+      <c r="A2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
+      <c r="A3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
+      <c r="A4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -413,7 +442,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Fix logs branch (#6)
* Fix log files
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jose</t>
   </si>
   <si>
     <t xml:space="preserve">customer</t>
@@ -191,13 +194,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -250,6 +253,23 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>654987</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -275,7 +295,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -353,17 +373,17 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -371,10 +391,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -402,11 +422,11 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -414,7 +434,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -422,15 +442,15 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>

</xml_diff>